<commit_message>
ajout d'un champ groupe_physique_id dans le model GroupePresntiel dans  + modification dans le controlleur GroupePresentielImportController + ajout d'un controlleur GroupePhysiqueImportController avec les veus necessaires et les routes necessaires + ajout d'un fichier excel GroupePH + modif d;un fichier excel GroupePR
</commit_message>
<xml_diff>
--- a/app/Fichiers Excel/GroupeDS.xlsx
+++ b/app/Fichiers Excel/GroupeDS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sora7\OneDrive\Desktop\Fichiers Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yacin\Desktop\eisgi_app\app\Fichiers Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C976B76-F6E0-4758-BFA6-1A6330417B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8040BC-892B-489D-A166-80B2FBB7E9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -648,21 +648,21 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E19"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="33.88671875" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" customWidth="1"/>
-    <col min="6" max="6" width="58.77734375" customWidth="1"/>
-    <col min="13" max="13" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="33.90625" customWidth="1"/>
+    <col min="3" max="3" width="27.90625" customWidth="1"/>
+    <col min="4" max="4" width="31.36328125" customWidth="1"/>
+    <col min="5" max="5" width="27.08984375" customWidth="1"/>
+    <col min="6" max="6" width="58.81640625" customWidth="1"/>
+    <col min="13" max="13" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -682,7 +682,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -705,7 +705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -728,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -751,7 +751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -774,7 +774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -797,7 +797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -820,7 +820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -843,7 +843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -866,7 +866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -889,7 +889,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -912,7 +912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -935,7 +935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -958,7 +958,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -981,7 +981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1096,177 +1096,177 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M29" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M32" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M38" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M54" t="s">
         <v>52</v>
       </c>

</xml_diff>